<commit_message>
adding materials for absolute size
</commit_message>
<xml_diff>
--- a/CATEGORIAL SIZE card sorting data/body_parts_cards.xlsx
+++ b/CATEGORIAL SIZE card sorting data/body_parts_cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/margaritapopova/Desktop/size matters/SizeMatters/CATEGORIAL SIZE card sorting data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF6C4870-5ADC-8545-A9BA-D6E000C0C3D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4407BF10-EE7B-CD4C-814E-79F1ED6F554D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="6500" windowWidth="23240" windowHeight="10340" xr2:uid="{3D187146-0FD7-4645-A6A8-B2334AF75869}"/>
+    <workbookView xWindow="5080" yWindow="4060" windowWidth="23240" windowHeight="10340" xr2:uid="{3D187146-0FD7-4645-A6A8-B2334AF75869}"/>
   </bookViews>
   <sheets>
     <sheet name="body ma c" sheetId="1" r:id="rId1"/>
@@ -523,7 +523,7 @@
   <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -866,5 +866,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>